<commit_message>
changes to main_task, part1_subj, segmentation, and data from first participant
</commit_message>
<xml_diff>
--- a/behavioral_August2019/psychopy experiment/audio_excel_sheets/31_audio.xlsx
+++ b/behavioral_August2019/psychopy experiment/audio_excel_sheets/31_audio.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="37">
   <si>
     <t>audio</t>
   </si>
@@ -123,9 +123,6 @@
   </si>
   <si>
     <t>parcelated_audio/31/31_36.aiff</t>
-  </si>
-  <si>
-    <t>parcelated_audio/31/31_37.aiff</t>
   </si>
 </sst>
 </file>
@@ -1437,7 +1434,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F38"/>
+  <dimension ref="A1:F37"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
       <pane topLeftCell="B2" xSplit="1" ySplit="1" activePane="bottomRight" state="frozen"/>
@@ -1824,16 +1821,6 @@
       <c r="E37" s="9"/>
       <c r="F37" s="9"/>
     </row>
-    <row r="38" ht="32.35" customHeight="1">
-      <c r="A38" t="s" s="7">
-        <v>37</v>
-      </c>
-      <c r="B38" s="8"/>
-      <c r="C38" s="9"/>
-      <c r="D38" s="9"/>
-      <c r="E38" s="9"/>
-      <c r="F38" s="9"/>
-    </row>
   </sheetData>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>

</xml_diff>